<commit_message>
[fix]convert psi value deg to rad
</commit_message>
<xml_diff>
--- a/general_python/datalist/20221110/TAKAOKI_swaytime_10-Nov-2022_10_56_40.xlsx
+++ b/general_python/datalist/20221110/TAKAOKI_swaytime_10-Nov-2022_10_56_40.xlsx
@@ -1,14 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fuekiyuuta/Documents/GitHub/hard_ware/general_python/datalist/20221110/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7646CAE2-5629-C343-81E9-7148FCA92CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -132,11 +152,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="Tsukushi A Round Gothic Bold"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,7 +173,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -155,69 +181,380 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL41"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="true"/>
-    <col min="2" max="2" width="12.42578125" customWidth="true"/>
-    <col min="3" max="3" width="7.7109375" customWidth="true"/>
-    <col min="4" max="4" width="12.42578125" customWidth="true"/>
-    <col min="5" max="5" width="9.28515625" customWidth="true"/>
-    <col min="6" max="6" width="12.7109375" customWidth="true"/>
-    <col min="7" max="7" width="12.7109375" customWidth="true"/>
-    <col min="8" max="8" width="16" customWidth="true"/>
-    <col min="9" max="9" width="17" customWidth="true"/>
-    <col min="10" max="10" width="12.85546875" customWidth="true"/>
-    <col min="11" max="11" width="14" customWidth="true"/>
-    <col min="12" max="12" width="8" customWidth="true"/>
-    <col min="13" max="13" width="13.7109375" customWidth="true"/>
-    <col min="14" max="14" width="17.7109375" customWidth="true"/>
-    <col min="15" max="15" width="17.42578125" customWidth="true"/>
-    <col min="16" max="16" width="16.42578125" customWidth="true"/>
-    <col min="17" max="17" width="13.5703125" customWidth="true"/>
-    <col min="18" max="18" width="12.42578125" customWidth="true"/>
-    <col min="19" max="19" width="11" customWidth="true"/>
-    <col min="20" max="20" width="12.42578125" customWidth="true"/>
-    <col min="21" max="21" width="12.5703125" customWidth="true"/>
-    <col min="22" max="22" width="14.7109375" customWidth="true"/>
-    <col min="23" max="23" width="12.7109375" customWidth="true"/>
-    <col min="24" max="24" width="12.42578125" customWidth="true"/>
-    <col min="25" max="25" width="11.140625" customWidth="true"/>
-    <col min="26" max="26" width="12.42578125" customWidth="true"/>
-    <col min="27" max="27" width="11" customWidth="true"/>
-    <col min="28" max="28" width="12.7109375" customWidth="true"/>
-    <col min="29" max="29" width="12.7109375" customWidth="true"/>
-    <col min="30" max="30" width="13.28515625" customWidth="true"/>
-    <col min="31" max="31" width="15.42578125" customWidth="true"/>
-    <col min="32" max="32" width="10.28515625" customWidth="true"/>
-    <col min="33" max="33" width="9.42578125" customWidth="true"/>
-    <col min="34" max="34" width="12.7109375" customWidth="true"/>
-    <col min="35" max="35" width="15.85546875" customWidth="true"/>
-    <col min="36" max="36" width="17.85546875" customWidth="true"/>
-    <col min="37" max="37" width="16.28515625" customWidth="true"/>
-    <col min="38" max="38" width="17.28515625" customWidth="true"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
+    <col min="15" max="15" width="17.5" customWidth="1"/>
+    <col min="16" max="16" width="16.5" customWidth="1"/>
+    <col min="17" max="17" width="13.5" customWidth="1"/>
+    <col min="18" max="18" width="12.5" customWidth="1"/>
+    <col min="19" max="19" width="11" customWidth="1"/>
+    <col min="20" max="21" width="12.5" customWidth="1"/>
+    <col min="22" max="22" width="14.6640625" customWidth="1"/>
+    <col min="23" max="23" width="12.6640625" customWidth="1"/>
+    <col min="24" max="24" width="12.5" customWidth="1"/>
+    <col min="25" max="25" width="11.1640625" customWidth="1"/>
+    <col min="26" max="26" width="12.5" customWidth="1"/>
+    <col min="27" max="27" width="11" customWidth="1"/>
+    <col min="28" max="29" width="12.6640625" customWidth="1"/>
+    <col min="30" max="30" width="13.33203125" customWidth="1"/>
+    <col min="31" max="31" width="15.5" customWidth="1"/>
+    <col min="32" max="32" width="10.33203125" customWidth="1"/>
+    <col min="33" max="33" width="9.5" customWidth="1"/>
+    <col min="34" max="34" width="12.6640625" customWidth="1"/>
+    <col min="35" max="35" width="15.83203125" customWidth="1"/>
+    <col min="36" max="36" width="17.83203125" customWidth="1"/>
+    <col min="37" max="37" width="16.33203125" customWidth="1"/>
+    <col min="38" max="38" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:38">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -333,7 +670,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:38">
       <c r="A2">
         <v>0</v>
       </c>
@@ -371,7 +708,7 @@
         <v>244</v>
       </c>
       <c r="M2">
-        <v>0.079999998211860657</v>
+        <v>7.9999998211860657E-2</v>
       </c>
       <c r="N2">
         <v>4</v>
@@ -389,13 +726,13 @@
         <v>-1.3861006498336792</v>
       </c>
       <c r="S2">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T2">
         <v>-1.2652082443237305</v>
       </c>
       <c r="U2">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V2">
         <v>-2.5103759765625</v>
@@ -425,7 +762,7 @@
         <v>1.0279395580291748</v>
       </c>
       <c r="AE2">
-        <v>0.0025699473917484283</v>
+        <v>2.5699473917484283E-3</v>
       </c>
       <c r="AF2">
         <v>0</v>
@@ -443,15 +780,15 @@
         <v>2.3700001239776611</v>
       </c>
       <c r="AK2">
-        <v>0.0025699473917484283</v>
+        <v>2.5699473917484283E-3</v>
       </c>
       <c r="AL2">
-        <v>-0.019200003147125333</v>
+        <v>-1.9200003147125333E-2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:38">
       <c r="A3">
-        <v>0.10000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="B3">
         <v>-1.3775242567062378</v>
@@ -466,7 +803,8 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.52759873867034912</v>
+        <f>F2+RADIANS(G2)+(A3-A2)</f>
+        <v>0.57060623701093771</v>
       </c>
       <c r="G3">
         <v>0.21711137890815735</v>
@@ -481,13 +819,13 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <v>244</v>
       </c>
       <c r="M3">
-        <v>0.079999998211860657</v>
+        <v>7.9999998211860657E-2</v>
       </c>
       <c r="N3">
         <v>4</v>
@@ -505,13 +843,13 @@
         <v>-1.386043906211853</v>
       </c>
       <c r="S3">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <v>-1.2638986110687256</v>
       </c>
       <c r="U3">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V3">
         <v>-2.39501953125</v>
@@ -541,7 +879,7 @@
         <v>1.0238481760025024</v>
       </c>
       <c r="AE3">
-        <v>0.0027841483242809772</v>
+        <v>2.7841483242809772E-3</v>
       </c>
       <c r="AF3">
         <v>0</v>
@@ -559,15 +897,15 @@
         <v>2.3700001239776611</v>
       </c>
       <c r="AK3">
-        <v>0.0027841483242809772</v>
+        <v>2.7841483242809772E-3</v>
       </c>
       <c r="AL3">
-        <v>-0.019200003147125333</v>
+        <v>-1.9200003147125333E-2</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:38">
       <c r="A4">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="B4">
         <v>-1.3798258304595947</v>
@@ -582,7 +920,8 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.58675605058670044</v>
+        <f t="shared" ref="F4:F41" si="0">F3+RADIANS(G3)+(A4-A3)</f>
+        <v>0.67439554541642999</v>
       </c>
       <c r="G4">
         <v>0.22059904038906097</v>
@@ -603,7 +942,7 @@
         <v>244</v>
       </c>
       <c r="M4">
-        <v>0.079999998211860657</v>
+        <v>7.9999998211860657E-2</v>
       </c>
       <c r="N4">
         <v>4</v>
@@ -621,13 +960,13 @@
         <v>-1.3857166767120361</v>
       </c>
       <c r="S4">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T4">
         <v>-1.2550761699676514</v>
       </c>
       <c r="U4">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V4">
         <v>-2.3345947265625</v>
@@ -657,7 +996,7 @@
         <v>1.0332802534103394</v>
       </c>
       <c r="AE4">
-        <v>0.0071021299809217453</v>
+        <v>7.1021299809217453E-3</v>
       </c>
       <c r="AF4">
         <v>0</v>
@@ -672,16 +1011,16 @@
         <v>1.0192999958992004</v>
       </c>
       <c r="AJ4">
-        <v>0.0099996849894523621</v>
+        <v>9.9996849894523621E-3</v>
       </c>
       <c r="AK4">
-        <v>0.0071021299809217453</v>
+        <v>7.1021299809217453E-3</v>
       </c>
       <c r="AL4">
-        <v>-0.019299995899200395</v>
+        <v>-1.9299995899200395E-2</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:38">
       <c r="A5">
         <v>0.30000000000000004</v>
       </c>
@@ -698,7 +1037,8 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.6462557315826416</v>
+        <f t="shared" si="0"/>
+        <v>0.77824572499795908</v>
       </c>
       <c r="G5">
         <v>0.22411274909973145</v>
@@ -719,7 +1059,7 @@
         <v>247</v>
       </c>
       <c r="M5">
-        <v>0.079999998211860657</v>
+        <v>7.9999998211860657E-2</v>
       </c>
       <c r="N5">
         <v>4</v>
@@ -737,13 +1077,13 @@
         <v>-1.3856625556945801</v>
       </c>
       <c r="S5">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T5">
         <v>-1.2537664175033569</v>
       </c>
       <c r="U5">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V5">
         <v>-2.2796630859375</v>
@@ -773,7 +1113,7 @@
         <v>1.0422393083572388</v>
       </c>
       <c r="AE5">
-        <v>0.0071074157021939754</v>
+        <v>7.1074157021939754E-3</v>
       </c>
       <c r="AF5">
         <v>0</v>
@@ -791,15 +1131,15 @@
         <v>-2.4699995517730713</v>
       </c>
       <c r="AK5">
-        <v>0.0071074157021939754</v>
+        <v>7.1074157021939754E-3</v>
       </c>
       <c r="AL5">
-        <v>0.0054000020027160645</v>
+        <v>5.4000020027160645E-3</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:38">
       <c r="A6">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="B6">
         <v>-1.3825641870498657</v>
@@ -814,7 +1154,8 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.70452135801315308</v>
+        <f t="shared" si="0"/>
+        <v>0.88215723036544536</v>
       </c>
       <c r="G6">
         <v>0.22783441841602325</v>
@@ -835,7 +1176,7 @@
         <v>247</v>
       </c>
       <c r="M6">
-        <v>0.079999998211860657</v>
+        <v>7.9999998211860657E-2</v>
       </c>
       <c r="N6">
         <v>4</v>
@@ -853,13 +1194,13 @@
         <v>-1.3856146335601807</v>
       </c>
       <c r="S6">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <v>-1.2525756359100342</v>
       </c>
       <c r="U6">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V6">
         <v>-2.2137451171875</v>
@@ -889,7 +1230,7 @@
         <v>1.0368410348892212</v>
       </c>
       <c r="AE6">
-        <v>0.0025889843236654997</v>
+        <v>2.5889843236654997E-3</v>
       </c>
       <c r="AF6">
         <v>0</v>
@@ -904,16 +1245,16 @@
         <v>0.99530000090599058</v>
       </c>
       <c r="AJ6">
-        <v>0.070000201463699341</v>
+        <v>7.0000201463699341E-2</v>
       </c>
       <c r="AK6">
-        <v>0.0025889843236654997</v>
+        <v>2.5889843236654997E-3</v>
       </c>
       <c r="AL6">
-        <v>0.0046999990940094216</v>
+        <v>4.6999990940094216E-3</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:38">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -930,7 +1271,8 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.7648543119430542</v>
+        <f t="shared" si="0"/>
+        <v>0.98613369111617133</v>
       </c>
       <c r="G7">
         <v>0.23188342154026031</v>
@@ -951,7 +1293,7 @@
         <v>250</v>
       </c>
       <c r="M7">
-        <v>0.070000000298023224</v>
+        <v>7.0000000298023224E-2</v>
       </c>
       <c r="N7">
         <v>4</v>
@@ -969,13 +1311,13 @@
         <v>-1.3855584859848022</v>
       </c>
       <c r="S7">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T7">
         <v>-1.251146674156189</v>
       </c>
       <c r="U7">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V7">
         <v>-2.1533203125</v>
@@ -1005,7 +1347,7 @@
         <v>1.0321381092071533</v>
       </c>
       <c r="AE7">
-        <v>0.0027119473088532686</v>
+        <v>2.7119473088532686E-3</v>
       </c>
       <c r="AF7">
         <v>0</v>
@@ -1023,13 +1365,13 @@
         <v>-2.3499996662139893</v>
       </c>
       <c r="AK7">
-        <v>0.0027119473088532686</v>
+        <v>2.7119473088532686E-3</v>
       </c>
       <c r="AL7">
-        <v>0.029299998283386253</v>
+        <v>2.9299998283386253E-2</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:38">
       <c r="A8">
         <v>0.60000000000000009</v>
       </c>
@@ -1046,7 +1388,8 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.82521206140518188</v>
+        <f t="shared" si="0"/>
+        <v>1.0901808203028389</v>
       </c>
       <c r="G8">
         <v>0.2358921617269516</v>
@@ -1067,7 +1410,7 @@
         <v>250</v>
       </c>
       <c r="M8">
-        <v>0.070000000298023224</v>
+        <v>7.0000000298023224E-2</v>
       </c>
       <c r="N8">
         <v>4</v>
@@ -1085,13 +1428,13 @@
         <v>-1.3855085372924805</v>
       </c>
       <c r="S8">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T8">
         <v>-1.249836802482605</v>
       </c>
       <c r="U8">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V8">
         <v>-2.08740234375</v>
@@ -1121,7 +1464,7 @@
         <v>1.027082085609436</v>
       </c>
       <c r="AE8">
-        <v>0.0025063520297408104</v>
+        <v>2.5063520297408104E-3</v>
       </c>
       <c r="AF8">
         <v>0</v>
@@ -1139,13 +1482,13 @@
         <v>-2.3499996662139893</v>
       </c>
       <c r="AK8">
-        <v>0.0025063520297408104</v>
+        <v>2.5063520297408104E-3</v>
       </c>
       <c r="AL8">
-        <v>0.029299998283386253</v>
+        <v>2.9299998283386253E-2</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:38">
       <c r="A9">
         <v>0.70000000000000007</v>
       </c>
@@ -1162,7 +1505,8 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.88707196712493896</v>
+        <f t="shared" si="0"/>
+        <v>1.1942979152046211</v>
       </c>
       <c r="G9">
         <v>0.24010391533374786</v>
@@ -1183,7 +1527,7 @@
         <v>250</v>
       </c>
       <c r="M9">
-        <v>0.070000000298023224</v>
+        <v>7.0000000298023224E-2</v>
       </c>
       <c r="N9">
         <v>4</v>
@@ -1201,13 +1545,13 @@
         <v>-1.3828147649765015</v>
       </c>
       <c r="S9">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T9">
         <v>-1.2496054172515869</v>
       </c>
       <c r="U9">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V9">
         <v>-2.021484375</v>
@@ -1237,7 +1581,7 @@
         <v>1.0091278553009033</v>
       </c>
       <c r="AE9">
-        <v>-0.0017847975250333548</v>
+        <v>-1.7847975250333548E-3</v>
       </c>
       <c r="AF9">
         <v>0</v>
@@ -1252,18 +1596,18 @@
         <v>0.99430000185966494</v>
       </c>
       <c r="AJ9">
-        <v>0.030000023543834686</v>
+        <v>3.0000023543834686E-2</v>
       </c>
       <c r="AK9">
-        <v>-0.0017847975250333548</v>
+        <v>-1.7847975250333548E-3</v>
       </c>
       <c r="AL9">
-        <v>0.0056999981403350608</v>
+        <v>5.6999981403350608E-3</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:38">
       <c r="A10">
-        <v>0.80000000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="B10">
         <v>-1.3839637041091919</v>
@@ -1278,7 +1622,8 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0.9500281810760498</v>
+        <f t="shared" si="0"/>
+        <v>1.2984885190741249</v>
       </c>
       <c r="G10">
         <v>0.24397012591362</v>
@@ -1299,7 +1644,7 @@
         <v>246</v>
       </c>
       <c r="M10">
-        <v>0.079999998211860657</v>
+        <v>7.9999998211860657E-2</v>
       </c>
       <c r="N10">
         <v>4</v>
@@ -1317,13 +1662,13 @@
         <v>-1.3854043483734131</v>
       </c>
       <c r="S10">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T10">
         <v>-1.2469786405563354</v>
       </c>
       <c r="U10">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V10">
         <v>-1.9610595703125</v>
@@ -1353,7 +1698,7 @@
         <v>1.0052503347396851</v>
       </c>
       <c r="AE10">
-        <v>0.0024685547687113285</v>
+        <v>2.4685547687113285E-3</v>
       </c>
       <c r="AF10">
         <v>0</v>
@@ -1368,18 +1713,18 @@
         <v>0.99430000185966494</v>
       </c>
       <c r="AJ10">
-        <v>0.030000023543834686</v>
+        <v>3.0000023543834686E-2</v>
       </c>
       <c r="AK10">
-        <v>0.0024685547687113285</v>
+        <v>2.4685547687113285E-3</v>
       </c>
       <c r="AL10">
-        <v>0.0056999981403350608</v>
+        <v>5.6999981403350608E-3</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:38">
       <c r="A11">
-        <v>0.90000000000000002</v>
+        <v>0.9</v>
       </c>
       <c r="B11">
         <v>-1.3843529224395752</v>
@@ -1394,7 +1739,8 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>1.0123004913330078</v>
+        <f t="shared" si="0"/>
+        <v>1.4027466010478227</v>
       </c>
       <c r="G11">
         <v>0.24773712456226349</v>
@@ -1415,7 +1761,7 @@
         <v>246</v>
       </c>
       <c r="M11">
-        <v>0.079999998211860657</v>
+        <v>7.9999998211860657E-2</v>
       </c>
       <c r="N11">
         <v>4</v>
@@ -1433,13 +1779,13 @@
         <v>-1.3853588104248047</v>
       </c>
       <c r="S11">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T11">
         <v>-1.2456685304641724</v>
       </c>
       <c r="U11">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V11">
         <v>-1.8951416015625</v>
@@ -1469,7 +1815,7 @@
         <v>1.0017585754394531</v>
       </c>
       <c r="AE11">
-        <v>0.002518774475902319</v>
+        <v>2.518774475902319E-3</v>
       </c>
       <c r="AF11">
         <v>0</v>
@@ -1487,13 +1833,13 @@
         <v>-2.6900002956390381</v>
       </c>
       <c r="AK11">
-        <v>0.002518774475902319</v>
+        <v>2.518774475902319E-3</v>
       </c>
       <c r="AL11">
-        <v>0.032599997520446733</v>
+        <v>3.2599997520446733E-2</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:38">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1504,13 +1850,14 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>-1.2501296997070313</v>
+        <v>-1.2501296997070312</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>1.0755577087402344</v>
+        <f t="shared" si="0"/>
+        <v>1.5070704295508577</v>
       </c>
       <c r="G12">
         <v>0.25146663188934326</v>
@@ -1531,7 +1878,7 @@
         <v>254</v>
       </c>
       <c r="M12">
-        <v>0.090000003576278687</v>
+        <v>9.0000003576278687E-2</v>
       </c>
       <c r="N12">
         <v>4</v>
@@ -1549,13 +1896,13 @@
         <v>-1.3882285356521606</v>
       </c>
       <c r="S12">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T12">
         <v>-1.2506734132766724</v>
       </c>
       <c r="U12">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V12">
         <v>-1.8951416015625</v>
@@ -1570,7 +1917,7 @@
         <v>0</v>
       </c>
       <c r="Z12">
-        <v>-1.2501296997070313</v>
+        <v>-1.2501296997070312</v>
       </c>
       <c r="AA12">
         <v>0</v>
@@ -1585,7 +1932,7 @@
         <v>0.98337382078170776</v>
       </c>
       <c r="AE12">
-        <v>-0.0023925849236547947</v>
+        <v>-2.3925849236547947E-3</v>
       </c>
       <c r="AF12">
         <v>0</v>
@@ -1603,13 +1950,13 @@
         <v>2.6199996471405029</v>
       </c>
       <c r="AK12">
-        <v>-0.0023925849236547947</v>
+        <v>-2.3925849236547947E-3</v>
       </c>
       <c r="AL12">
-        <v>0.0083200013637543258</v>
+        <v>8.3200013637543258E-3</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:38">
       <c r="A13">
         <v>1.1000000000000001</v>
       </c>
@@ -1626,7 +1973,8 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>1.1380497217178345</v>
+        <f t="shared" si="0"/>
+        <v>1.6114593502362273</v>
       </c>
       <c r="G13">
         <v>0.25509831309318542</v>
@@ -1647,7 +1995,7 @@
         <v>254</v>
       </c>
       <c r="M13">
-        <v>0.090000003576278687</v>
+        <v>9.0000003576278687E-2</v>
       </c>
       <c r="N13">
         <v>4</v>
@@ -1665,13 +2013,13 @@
         <v>-1.388185977935791</v>
       </c>
       <c r="S13">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T13">
         <v>-1.2493631839752197</v>
       </c>
       <c r="U13">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V13">
         <v>-1.834716796875</v>
@@ -1701,7 +2049,7 @@
         <v>0.9807165265083313</v>
       </c>
       <c r="AE13">
-        <v>0.0023908577859401703</v>
+        <v>2.3908577859401703E-3</v>
       </c>
       <c r="AF13">
         <v>0</v>
@@ -1716,16 +2064,16 @@
         <v>1.010880001783371</v>
       </c>
       <c r="AJ13">
-        <v>1.0490417423625331e-07</v>
+        <v>1.0490417423625331E-7</v>
       </c>
       <c r="AK13">
-        <v>0.0023908577859401703</v>
+        <v>2.3908577859401703E-3</v>
       </c>
       <c r="AL13">
-        <v>0.0083200013637543258</v>
+        <v>8.3200013637543258E-3</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:38">
       <c r="A14">
         <v>1.2000000000000002</v>
       </c>
@@ -1742,7 +2090,8 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>1.2615092992782593</v>
+        <f t="shared" si="0"/>
+        <v>1.7159116557159868</v>
       </c>
       <c r="G14">
         <v>0.26164934039115906</v>
@@ -1763,7 +2112,7 @@
         <v>254</v>
       </c>
       <c r="M14">
-        <v>0.090000003576278687</v>
+        <v>9.0000003576278687E-2</v>
       </c>
       <c r="N14">
         <v>4</v>
@@ -1781,13 +2130,13 @@
         <v>-1.3910624980926514</v>
       </c>
       <c r="S14">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T14">
         <v>-1.2544870376586914</v>
       </c>
       <c r="U14">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V14">
         <v>-1.7138671875</v>
@@ -1817,7 +2166,7 @@
         <v>0.9623224139213562</v>
       </c>
       <c r="AE14">
-        <v>-0.0020138791296631098</v>
+        <v>-2.0138791296631098E-3</v>
       </c>
       <c r="AF14">
         <v>0</v>
@@ -1835,13 +2184,13 @@
         <v>2.3400001525878906</v>
       </c>
       <c r="AK14">
-        <v>-0.0020138791296631098</v>
+        <v>-2.0138791296631098E-3</v>
       </c>
       <c r="AL14">
-        <v>0.0090299975872041305</v>
+        <v>9.0299975872041305E-3</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:38">
       <c r="A15">
         <v>1.3</v>
       </c>
@@ -1858,7 +2207,8 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>1.3227376937866211</v>
+        <f t="shared" si="0"/>
+        <v>1.8204782981914838</v>
       </c>
       <c r="G15">
         <v>0.26517972350120544</v>
@@ -1897,13 +2247,13 @@
         <v>-1.3910225629806519</v>
       </c>
       <c r="S15">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T15">
         <v>-1.2531768083572388</v>
       </c>
       <c r="U15">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V15">
         <v>-1.6534423828125</v>
@@ -1933,7 +2283,7 @@
         <v>0.96045327186584473</v>
       </c>
       <c r="AE15">
-        <v>0.0022581324446946383</v>
+        <v>2.2581324446946383E-3</v>
       </c>
       <c r="AF15">
         <v>0</v>
@@ -1948,16 +2298,16 @@
         <v>0.98873999714851379</v>
       </c>
       <c r="AJ15">
-        <v>0.069999799132347107</v>
+        <v>6.9999799132347107E-2</v>
       </c>
       <c r="AK15">
-        <v>0.0022581324446946383</v>
+        <v>2.2581324446946383E-3</v>
       </c>
       <c r="AL15">
-        <v>0.0058600008487701416</v>
+        <v>5.8600008487701416E-3</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:38">
       <c r="A16">
         <v>1.4000000000000001</v>
       </c>
@@ -1974,7 +2324,8 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>1.3227376937866211</v>
+        <f t="shared" si="0"/>
+        <v>1.9251065574761081</v>
       </c>
       <c r="G16">
         <v>0.26517972350120544</v>
@@ -2013,13 +2364,13 @@
         <v>-1.390984058380127</v>
       </c>
       <c r="S16">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T16">
         <v>-1.2518664598464966</v>
       </c>
       <c r="U16">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V16">
         <v>-1.5875244140625</v>
@@ -2049,7 +2400,7 @@
         <v>0.96045327186584473</v>
       </c>
       <c r="AE16">
-        <v>0.0022581324446946383</v>
+        <v>2.2581324446946383E-3</v>
       </c>
       <c r="AF16">
         <v>0</v>
@@ -2067,13 +2418,13 @@
         <v>-2.4599997997283936</v>
       </c>
       <c r="AK16">
-        <v>0.0022581324446946383</v>
+        <v>2.2581324446946383E-3</v>
       </c>
       <c r="AL16">
-        <v>0.030530000329017537</v>
+        <v>3.0530000329017537E-2</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:38">
       <c r="A17">
         <v>1.5</v>
       </c>
@@ -2090,7 +2441,8 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>1.3852331638336182</v>
+        <f t="shared" si="0"/>
+        <v>2.0297348167607323</v>
       </c>
       <c r="G17">
         <v>0.26916080713272095</v>
@@ -2129,13 +2481,13 @@
         <v>-1.3909436464309692</v>
       </c>
       <c r="S17">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T17">
         <v>-1.2504370212554932</v>
       </c>
       <c r="U17">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V17">
         <v>-1.5216064453125</v>
@@ -2165,7 +2517,7 @@
         <v>0.95908164978027344</v>
       </c>
       <c r="AE17">
-        <v>0.0023816982284188271</v>
+        <v>2.3816982284188271E-3</v>
       </c>
       <c r="AF17">
         <v>0</v>
@@ -2183,15 +2535,15 @@
         <v>-2.4599997997283936</v>
       </c>
       <c r="AK17">
-        <v>0.0023816982284188271</v>
+        <v>2.3816982284188271E-3</v>
       </c>
       <c r="AL17">
-        <v>0.028070000410079898</v>
+        <v>2.8070000410079898E-2</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:38">
       <c r="A18">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="B18">
         <v>-1.3896571397781372</v>
@@ -2206,7 +2558,8 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>1.4486531019210815</v>
+        <f t="shared" si="0"/>
+        <v>2.1344325590625237</v>
       </c>
       <c r="G18">
         <v>0.27346664667129517</v>
@@ -2245,13 +2598,13 @@
         <v>-1.3909049034118652</v>
       </c>
       <c r="S18">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T18">
         <v>-1.2490074634552002</v>
       </c>
       <c r="U18">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V18">
         <v>-1.4501953125</v>
@@ -2281,7 +2634,7 @@
         <v>0.94398820400238037</v>
       </c>
       <c r="AE18">
-        <v>-0.00210987264290452</v>
+        <v>-2.10987264290452E-3</v>
       </c>
       <c r="AF18">
         <v>0</v>
@@ -2299,13 +2652,13 @@
         <v>-0.29999998211860657</v>
       </c>
       <c r="AK18">
-        <v>-0.00210987264290452</v>
+        <v>-2.10987264290452E-3</v>
       </c>
       <c r="AL18">
-        <v>0.0060699975490569047</v>
+        <v>6.0699975490569047E-3</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:38">
       <c r="A19">
         <v>1.7000000000000002</v>
       </c>
@@ -2322,7 +2675,8 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>1.5142320394515991</v>
+        <f t="shared" si="0"/>
+        <v>2.2392054524413258</v>
       </c>
       <c r="G19">
         <v>0.27797257900238037</v>
@@ -2361,13 +2715,13 @@
         <v>-1.3908647298812866</v>
       </c>
       <c r="S19">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T19">
         <v>-1.2474586963653564</v>
       </c>
       <c r="U19">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V19">
         <v>-1.3787841796875</v>
@@ -2397,7 +2751,7 @@
         <v>0.94376450777053833</v>
       </c>
       <c r="AE19">
-        <v>0.0024541658349335194</v>
+        <v>2.4541658349335194E-3</v>
       </c>
       <c r="AF19">
         <v>0</v>
@@ -2415,13 +2769,13 @@
         <v>-0.29999998211860657</v>
       </c>
       <c r="AK19">
-        <v>0.0024541658349335194</v>
+        <v>2.4541658349335194E-3</v>
       </c>
       <c r="AL19">
-        <v>0.0084299975633621571</v>
+        <v>8.4299975633621571E-3</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:38">
       <c r="A20">
         <v>1.8</v>
       </c>
@@ -2438,7 +2792,8 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>1.5813864469528198</v>
+        <f t="shared" si="0"/>
+        <v>2.3440569891751775</v>
       </c>
       <c r="G20">
         <v>0.28267660737037659</v>
@@ -2477,13 +2832,13 @@
         <v>-1.3879085779190063</v>
       </c>
       <c r="S20">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T20">
         <v>-1.2394758462905884</v>
       </c>
       <c r="U20">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V20">
         <v>-1.3018798828125</v>
@@ -2513,7 +2868,7 @@
         <v>0.94187057018280029</v>
       </c>
       <c r="AE20">
-        <v>0.0019024665234610438</v>
+        <v>1.9024665234610438E-3</v>
       </c>
       <c r="AF20">
         <v>0</v>
@@ -2528,16 +2883,16 @@
         <v>0.9866699999570846</v>
       </c>
       <c r="AJ20">
-        <v>0.079999737441539764</v>
+        <v>7.9999737441539764E-2</v>
       </c>
       <c r="AK20">
-        <v>0.0019024665234610438</v>
+        <v>1.9024665234610438E-3</v>
       </c>
       <c r="AL20">
-        <v>0.0076300019025803412</v>
+        <v>7.6300019025803412E-3</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:38">
       <c r="A21">
         <v>1.9000000000000001</v>
       </c>
@@ -2554,7 +2909,8 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>1.6511749029159546</v>
+        <f t="shared" si="0"/>
+        <v>2.4489906266921579</v>
       </c>
       <c r="G21">
         <v>0.28721234202384949</v>
@@ -2593,13 +2949,13 @@
         <v>-1.3934283256530762</v>
       </c>
       <c r="S21">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T21">
         <v>-1.243044376373291</v>
       </c>
       <c r="U21">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V21">
         <v>-1.3018798828125</v>
@@ -2629,7 +2985,7 @@
         <v>0.94053161144256592</v>
       </c>
       <c r="AE21">
-        <v>0.0020449219737201929</v>
+        <v>2.0449219737201929E-3</v>
       </c>
       <c r="AF21">
         <v>0</v>
@@ -2647,13 +3003,13 @@
         <v>0.11000017076730728</v>
       </c>
       <c r="AK21">
-        <v>0.0020449219737201929</v>
+        <v>2.0449219737201929E-3</v>
       </c>
       <c r="AL21">
-        <v>0.0038399982452391734</v>
+        <v>3.8399982452391734E-3</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:38">
       <c r="A22">
         <v>2</v>
       </c>
@@ -2670,7 +3026,8 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>1.7228857278823853</v>
+        <f t="shared" si="0"/>
+        <v>2.5540034277128383</v>
       </c>
       <c r="G22">
         <v>0.29200661182403564</v>
@@ -2709,13 +3066,13 @@
         <v>-1.3933916091918945</v>
       </c>
       <c r="S22">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T22">
         <v>-1.2413763999938965</v>
       </c>
       <c r="U22">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V22">
         <v>-1.2249755859375</v>
@@ -2745,7 +3102,7 @@
         <v>0.93988478183746338</v>
       </c>
       <c r="AE22">
-        <v>0.0022418403532356024</v>
+        <v>2.2418403532356024E-3</v>
       </c>
       <c r="AF22">
         <v>0</v>
@@ -2763,15 +3120,15 @@
         <v>-2.4500002861022949</v>
       </c>
       <c r="AK22">
-        <v>0.0022418403532356024</v>
+        <v>2.2418403532356024E-3</v>
       </c>
       <c r="AL22">
-        <v>0.032687998652458305</v>
+        <v>3.2687998652458305E-2</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:38">
       <c r="A23">
-        <v>2.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="B23">
         <v>-1.3913804292678833</v>
@@ -2786,7 +3143,8 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>1.7959996461868286</v>
+        <f t="shared" si="0"/>
+        <v>2.6590999045267609</v>
       </c>
       <c r="G23">
         <v>0.29651027917861938</v>
@@ -2825,13 +3183,13 @@
         <v>-1.3933570384979248</v>
       </c>
       <c r="S23">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T23">
         <v>-1.239708423614502</v>
       </c>
       <c r="U23">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V23">
         <v>-1.1480712890625</v>
@@ -2861,7 +3219,7 @@
         <v>0.92553156614303589</v>
       </c>
       <c r="AE23">
-        <v>-0.0022312353830784559</v>
+        <v>-2.2312353830784559E-3</v>
       </c>
       <c r="AF23">
         <v>0</v>
@@ -2879,13 +3237,13 @@
         <v>0.15999984741210938</v>
       </c>
       <c r="AK23">
-        <v>-0.0022312353830784559</v>
+        <v>-2.2312353830784559E-3</v>
       </c>
       <c r="AL23">
-        <v>0.031088001370430107</v>
+        <v>3.1088001370430107E-2</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:38">
       <c r="A24">
         <v>2.2000000000000002</v>
       </c>
@@ -2902,7 +3260,8 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>1.8686535358428955</v>
+        <f t="shared" si="0"/>
+        <v>2.7642749851644357</v>
       </c>
       <c r="G24">
         <v>0.3006654679775238</v>
@@ -2941,13 +3300,13 @@
         <v>-1.393326997756958</v>
       </c>
       <c r="S24">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T24">
         <v>-1.2381594181060791</v>
       </c>
       <c r="U24">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V24">
         <v>-1.07666015625</v>
@@ -2977,7 +3336,7 @@
         <v>0.91288095712661743</v>
       </c>
       <c r="AE24">
-        <v>-0.0019353136885911226</v>
+        <v>-1.9353136885911226E-3</v>
       </c>
       <c r="AF24">
         <v>0</v>
@@ -2995,13 +3354,13 @@
         <v>2.3700001239776611</v>
       </c>
       <c r="AK24">
-        <v>-0.0019353136885911226</v>
+        <v>-1.9353136885911226E-3</v>
       </c>
       <c r="AL24">
-        <v>0.0073270021677016572</v>
+        <v>7.3270021677016572E-3</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:38">
       <c r="A25">
         <v>2.3000000000000003</v>
       </c>
@@ -3018,7 +3377,8 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>1.9409717321395874</v>
+        <f t="shared" si="0"/>
+        <v>2.8695225875276931</v>
       </c>
       <c r="G25">
         <v>0.30496147274971008</v>
@@ -3057,13 +3417,13 @@
         <v>-1.3962166309356689</v>
       </c>
       <c r="S25">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T25">
         <v>-1.2430446147918701</v>
       </c>
       <c r="U25">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V25">
         <v>-1.0052490234375</v>
@@ -3093,7 +3453,7 @@
         <v>0.91423386335372925</v>
       </c>
       <c r="AE25">
-        <v>0.0023912766482681036</v>
+        <v>2.3912766482681036E-3</v>
       </c>
       <c r="AF25">
         <v>0</v>
@@ -3111,13 +3471,13 @@
         <v>-0.13999976217746735</v>
       </c>
       <c r="AK25">
-        <v>0.0023912766482681036</v>
+        <v>2.3912766482681036E-3</v>
       </c>
       <c r="AL25">
-        <v>0.0065740019083022627</v>
+        <v>6.5740019083022627E-3</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:38">
       <c r="A26">
         <v>2.4000000000000004</v>
       </c>
@@ -3134,7 +3494,8 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>2.014528751373291</v>
+        <f t="shared" si="0"/>
+        <v>2.9748451693189066</v>
       </c>
       <c r="G26">
         <v>0.30903258919715881</v>
@@ -3173,13 +3534,13 @@
         <v>-1.3991063833236694</v>
       </c>
       <c r="S26">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T26">
         <v>-1.2478104829788208</v>
       </c>
       <c r="U26">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V26">
         <v>-0.9283447265625</v>
@@ -3209,7 +3570,7 @@
         <v>0.91472554206848145</v>
       </c>
       <c r="AE26">
-        <v>0.0021315447520464659</v>
+        <v>2.1315447520464659E-3</v>
       </c>
       <c r="AF26">
         <v>0</v>
@@ -3224,16 +3585,16 @@
         <v>0.9611930025219918</v>
       </c>
       <c r="AJ26">
-        <v>0.060000218451023102</v>
+        <v>6.0000218451023102E-2</v>
       </c>
       <c r="AK26">
-        <v>0.0021315447520464659</v>
+        <v>2.1315447520464659E-3</v>
       </c>
       <c r="AL26">
-        <v>0.0035769980549812397</v>
+        <v>3.5769980549812397E-3</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:38">
       <c r="A27">
         <v>2.5</v>
       </c>
@@ -3250,7 +3611,8 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>2.0875060558319092</v>
+        <f t="shared" si="0"/>
+        <v>3.0802388054963599</v>
       </c>
       <c r="G27">
         <v>0.31324535608291626</v>
@@ -3289,13 +3651,13 @@
         <v>-1.3964413404464722</v>
       </c>
       <c r="S27">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T27">
         <v>-1.2474591732025146</v>
       </c>
       <c r="U27">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V27">
         <v>-0.85693359375</v>
@@ -3325,7 +3687,7 @@
         <v>0.91552627086639404</v>
       </c>
       <c r="AE27">
-        <v>0.0022371015511453152</v>
+        <v>2.2371015511453152E-3</v>
       </c>
       <c r="AF27">
         <v>0</v>
@@ -3340,18 +3702,18 @@
         <v>0.94106699979305264</v>
       </c>
       <c r="AJ27">
-        <v>-0.020000200718641281</v>
+        <v>-2.0000200718641281E-2</v>
       </c>
       <c r="AK27">
-        <v>0.0022371015511453152</v>
+        <v>2.2371015511453152E-3</v>
       </c>
       <c r="AL27">
-        <v>0.0015630015134812103</v>
+        <v>1.5630015134812103E-3</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:38">
       <c r="A28">
-        <v>2.6000000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="B28">
         <v>-1.3953229188919067</v>
@@ -3366,7 +3728,8 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <v>2.1600604057312012</v>
+        <f t="shared" si="0"/>
+        <v>3.1857059683265887</v>
       </c>
       <c r="G28">
         <v>0.31759840250015259</v>
@@ -3405,13 +3768,13 @@
         <v>-1.3964190483093262</v>
       </c>
       <c r="S28">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T28">
         <v>-1.2459100484848022</v>
       </c>
       <c r="U28">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V28">
         <v>-0.7855224609375</v>
@@ -3441,7 +3804,7 @@
         <v>0.91616982221603394</v>
       </c>
       <c r="AE28">
-        <v>0.0021965389605611563</v>
+        <v>2.1965389605611563E-3</v>
       </c>
       <c r="AF28">
         <v>0</v>
@@ -3459,15 +3822,15 @@
         <v>0.15000014007091522</v>
       </c>
       <c r="AK28">
-        <v>0.0021965389605611563</v>
+        <v>2.1965389605611563E-3</v>
       </c>
       <c r="AL28">
-        <v>0.0022630032300949843</v>
+        <v>2.2630032300949843E-3</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:38">
       <c r="A29">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="B29">
         <v>-1.3956190347671509</v>
@@ -3482,7 +3845,8 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>2.2337899208068848</v>
+        <f t="shared" si="0"/>
+        <v>3.2912491061492908</v>
       </c>
       <c r="G29">
         <v>0.3221510648727417</v>
@@ -3521,13 +3885,13 @@
         <v>-1.3937563896179199</v>
       </c>
       <c r="S29">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T29">
         <v>-1.2454395294189453</v>
       </c>
       <c r="U29">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V29">
         <v>-0.7086181640625</v>
@@ -3557,7 +3921,7 @@
         <v>0.91761869192123413</v>
       </c>
       <c r="AE29">
-        <v>0.0024661440402269363</v>
+        <v>2.4661440402269363E-3</v>
       </c>
       <c r="AF29">
         <v>0</v>
@@ -3572,16 +3936,16 @@
         <v>0.98068300539255149</v>
       </c>
       <c r="AJ29">
-        <v>-0.079999715089797974</v>
+        <v>-7.9999715089797974E-2</v>
       </c>
       <c r="AK29">
-        <v>0.0024661440402269363</v>
+        <v>2.4661440402269363E-3</v>
       </c>
       <c r="AL29">
-        <v>0.0051869989037512942</v>
+        <v>5.1869989037512942E-3</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:38">
       <c r="A30">
         <v>2.8000000000000003</v>
       </c>
@@ -3598,7 +3962,8 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>2.3083770275115967</v>
+        <f t="shared" si="0"/>
+        <v>3.3968717029201261</v>
       </c>
       <c r="G30">
         <v>0.3268406093120575</v>
@@ -3637,13 +4002,13 @@
         <v>-1.3937368392944336</v>
       </c>
       <c r="S30">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T30">
         <v>-1.2437711954116821</v>
       </c>
       <c r="U30">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V30">
         <v>-0.6317138671875</v>
@@ -3673,7 +4038,7 @@
         <v>0.91853755712509155</v>
       </c>
       <c r="AE30">
-        <v>0.0023157200776040554</v>
+        <v>2.3157200776040554E-3</v>
       </c>
       <c r="AF30">
         <v>0</v>
@@ -3691,13 +4056,13 @@
         <v>-2.4200000762939453</v>
       </c>
       <c r="AK30">
-        <v>0.0023157200776040554</v>
+        <v>2.3157200776040554E-3</v>
       </c>
       <c r="AL30">
-        <v>0.029467002809047682</v>
+        <v>2.9467002809047682E-2</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:38">
       <c r="A31">
         <v>2.9000000000000004</v>
       </c>
@@ -3714,7 +4079,8 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>2.3850741386413574</v>
+        <f t="shared" si="0"/>
+        <v>3.5025761476818462</v>
       </c>
       <c r="G31">
         <v>0.33154425024986267</v>
@@ -3753,13 +4119,13 @@
         <v>-1.3963594436645508</v>
       </c>
       <c r="S31">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T31">
         <v>-1.240786075592041</v>
       </c>
       <c r="U31">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V31">
         <v>-0.54931640625</v>
@@ -3789,7 +4155,7 @@
         <v>0.90583056211471558</v>
       </c>
       <c r="AE31">
-        <v>-0.0021027680486440659</v>
+        <v>-2.1027680486440659E-3</v>
       </c>
       <c r="AF31">
         <v>0</v>
@@ -3807,13 +4173,13 @@
         <v>2.4700002670288086</v>
       </c>
       <c r="AK31">
-        <v>-0.0021027680486440659</v>
+        <v>-2.1027680486440659E-3</v>
       </c>
       <c r="AL31">
-        <v>0.0024559993743896724</v>
+        <v>2.4559993743896724E-3</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:38">
       <c r="A32">
         <v>3</v>
       </c>
@@ -3830,7 +4196,8 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>2.4633111953735352</v>
+        <f t="shared" si="0"/>
+        <v>3.608362686464762</v>
       </c>
       <c r="G32">
         <v>0.33656543493270874</v>
@@ -3869,13 +4236,13 @@
         <v>-1.3963435888290405</v>
       </c>
       <c r="S32">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T32">
         <v>-1.2389985322952271</v>
       </c>
       <c r="U32">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V32">
         <v>-0.4669189453125</v>
@@ -3905,7 +4272,7 @@
         <v>0.90769112110137939</v>
       </c>
       <c r="AE32">
-        <v>0.0024065356701612473</v>
+        <v>2.4065356701612473E-3</v>
       </c>
       <c r="AF32">
         <v>0</v>
@@ -3920,18 +4287,18 @@
         <v>0.97357280095815657</v>
       </c>
       <c r="AJ32">
-        <v>-0.070000104606151581</v>
+        <v>-7.0000104606151581E-2</v>
       </c>
       <c r="AK32">
-        <v>0.0024065356701612473</v>
+        <v>2.4065356701612473E-3</v>
       </c>
       <c r="AL32">
-        <v>0.0046192021727561317</v>
+        <v>4.6192021727561317E-3</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:38">
       <c r="A33">
-        <v>3.1000000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="B33">
         <v>-1.3954943418502808</v>
@@ -3946,7 +4313,8 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>2.5426723957061768</v>
+        <f t="shared" si="0"/>
+        <v>3.7142368614527448</v>
       </c>
       <c r="G33">
         <v>0.34135448932647705</v>
@@ -3985,13 +4353,13 @@
         <v>-1.3963302373886108</v>
       </c>
       <c r="S33">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T33">
         <v>-1.2372111082077026</v>
       </c>
       <c r="U33">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V33">
         <v>-0.384521484375</v>
@@ -4021,7 +4389,7 @@
         <v>0.90905463695526123</v>
       </c>
       <c r="AE33">
-        <v>0.0022744606249034405</v>
+        <v>2.2744606249034405E-3</v>
       </c>
       <c r="AF33">
         <v>0</v>
@@ -4039,15 +4407,15 @@
         <v>-2.2699997425079346</v>
       </c>
       <c r="AK33">
-        <v>0.0022744606249034405</v>
+        <v>2.2744606249034405E-3</v>
       </c>
       <c r="AL33">
-        <v>0.02747920171022411</v>
+        <v>2.747920171022411E-2</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:38">
       <c r="A34">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="B34">
         <v>-1.3957201242446899</v>
@@ -4062,7 +4430,8 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>2.6213696002960205</v>
+        <f t="shared" si="0"/>
+        <v>3.8201946212079556</v>
       </c>
       <c r="G34">
         <v>0.34591370820999146</v>
@@ -4101,13 +4470,13 @@
         <v>-1.3989611864089966</v>
       </c>
       <c r="S34">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T34">
         <v>-1.2343450784683228</v>
       </c>
       <c r="U34">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V34">
         <v>-0.3076171875</v>
@@ -4137,7 +4506,7 @@
         <v>0.89760869741439819</v>
       </c>
       <c r="AE34">
-        <v>-0.0018703402020037174</v>
+        <v>-1.8703402020037174E-3</v>
       </c>
       <c r="AF34">
         <v>0</v>
@@ -4155,13 +4524,13 @@
         <v>2.3100001811981201</v>
       </c>
       <c r="AK34">
-        <v>-0.0018703402020037174</v>
+        <v>-1.8703402020037174E-3</v>
       </c>
       <c r="AL34">
-        <v>0.0066943006634712088</v>
+        <v>6.6943006634712088E-3</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:38">
       <c r="A35">
         <v>3.3000000000000003</v>
       </c>
@@ -4178,7 +4547,8 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>2.7010667324066162</v>
+        <f t="shared" si="0"/>
+        <v>3.926231954344003</v>
       </c>
       <c r="G35">
         <v>0.35030609369277954</v>
@@ -4217,13 +4587,13 @@
         <v>-1.39631187915802</v>
       </c>
       <c r="S35">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T35">
         <v>-1.2337551116943359</v>
       </c>
       <c r="U35">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V35">
         <v>-0.2252197265625</v>
@@ -4253,7 +4623,7 @@
         <v>0.89976221323013306</v>
       </c>
       <c r="AE35">
-        <v>0.002346687251701951</v>
+        <v>2.346687251701951E-3</v>
       </c>
       <c r="AF35">
         <v>0</v>
@@ -4271,13 +4641,13 @@
         <v>-0.11999989300966263</v>
       </c>
       <c r="AK35">
-        <v>0.002346687251701951</v>
+        <v>2.346687251701951E-3</v>
       </c>
       <c r="AL35">
-        <v>0.0058165970444679083</v>
+        <v>5.8165970444679083E-3</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:38">
       <c r="A36">
         <v>3.4000000000000004</v>
       </c>
@@ -4294,7 +4664,8 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>2.7800090312957764</v>
+        <f t="shared" si="0"/>
+        <v>4.0323459490687412</v>
       </c>
       <c r="G36">
         <v>0.35459402203559875</v>
@@ -4333,13 +4704,13 @@
         <v>-1.3963063955307007</v>
       </c>
       <c r="S36">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T36">
         <v>-1.2320867776870728</v>
       </c>
       <c r="U36">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V36">
         <v>-0.1483154296875</v>
@@ -4369,7 +4740,7 @@
         <v>0.90112173557281494</v>
       </c>
       <c r="AE36">
-        <v>0.0021235176827758551</v>
+        <v>2.1235176827758551E-3</v>
       </c>
       <c r="AF36">
         <v>0</v>
@@ -4387,13 +4758,13 @@
         <v>-2.2400002479553223</v>
       </c>
       <c r="AK36">
-        <v>0.0021235176827758551</v>
+        <v>2.1235176827758551E-3</v>
       </c>
       <c r="AL36">
-        <v>0.026119301444292087</v>
+        <v>2.6119301444292087E-2</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:38">
       <c r="A37">
         <v>3.5</v>
       </c>
@@ -4410,7 +4781,8 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>2.8584010601043701</v>
+        <f t="shared" si="0"/>
+        <v>4.1385347822611518</v>
       </c>
       <c r="G37">
         <v>0.35853564739227295</v>
@@ -4449,16 +4821,16 @@
         <v>-1.3910213708877563</v>
       </c>
       <c r="S37">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T37">
         <v>-1.2328137159347534</v>
       </c>
       <c r="U37">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V37">
-        <v>-0.0714111328125</v>
+        <v>-7.14111328125E-2</v>
       </c>
       <c r="W37">
         <v>0.750732421875</v>
@@ -4485,7 +4857,7 @@
         <v>0.88984036445617676</v>
       </c>
       <c r="AE37">
-        <v>-0.0019662862177938223</v>
+        <v>-1.9662862177938223E-3</v>
       </c>
       <c r="AF37">
         <v>0</v>
@@ -4503,15 +4875,15 @@
         <v>0.16000011563301086</v>
       </c>
       <c r="AK37">
-        <v>-0.0019662862177938223</v>
+        <v>-1.9662862177938223E-3</v>
       </c>
       <c r="AL37">
-        <v>0.022506697928905584</v>
+        <v>2.2506697928905584E-2</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:38">
       <c r="A38">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="B38">
         <v>-1.3949918746948242</v>
@@ -4526,7 +4898,8 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>2.9363911151885986</v>
+        <f t="shared" si="0"/>
+        <v>4.2447924097939165</v>
       </c>
       <c r="G38">
         <v>0.36231660842895508</v>
@@ -4565,16 +4938,16 @@
         <v>-1.3883794546127319</v>
       </c>
       <c r="S38">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T38">
         <v>-1.2323429584503174</v>
       </c>
       <c r="U38">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V38">
-        <v>0.0054931640625</v>
+        <v>5.4931640625E-3</v>
       </c>
       <c r="W38">
         <v>0.738525390625</v>
@@ -4601,7 +4974,7 @@
         <v>0.88008922338485718</v>
       </c>
       <c r="AE38">
-        <v>-0.0016708472976461053</v>
+        <v>-1.6708472976461053E-3</v>
       </c>
       <c r="AF38">
         <v>0</v>
@@ -4619,15 +4992,15 @@
         <v>2.2499997615814209</v>
       </c>
       <c r="AK38">
-        <v>-0.0016708472976461053</v>
+        <v>-1.6708472976461053E-3</v>
       </c>
       <c r="AL38">
-        <v>0.0021367016196250921</v>
+        <v>2.1367016196250921E-3</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:38">
       <c r="A39">
-        <v>3.7000000000000002</v>
+        <v>3.7</v>
       </c>
       <c r="B39">
         <v>-1.3932055234909058</v>
@@ -4642,7 +5015,8 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <v>3.012603759765625</v>
+        <f t="shared" si="0"/>
+        <v>4.3511160275456611</v>
       </c>
       <c r="G39">
         <v>0.3659384548664093</v>
@@ -4681,16 +5055,16 @@
         <v>-1.3886574506759644</v>
       </c>
       <c r="S39">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T39">
         <v>-1.2384254932403564</v>
       </c>
       <c r="U39">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V39">
-        <v>0.076904296875</v>
+        <v>7.6904296875E-2</v>
       </c>
       <c r="W39">
         <v>0.726318359375</v>
@@ -4717,7 +5091,7 @@
         <v>0.88350582122802734</v>
       </c>
       <c r="AE39">
-        <v>0.0024363710545003414</v>
+        <v>2.4363710545003414E-3</v>
       </c>
       <c r="AF39">
         <v>0</v>
@@ -4735,13 +5109,13 @@
         <v>2.2600002288818359</v>
       </c>
       <c r="AK39">
-        <v>0.0024363710545003414</v>
+        <v>2.4363710545003414E-3</v>
       </c>
       <c r="AL39">
-        <v>-0.018631704992055909</v>
+        <v>-1.8631704992055909E-2</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:38">
       <c r="A40">
         <v>3.8000000000000003</v>
       </c>
@@ -4758,7 +5132,8 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>3.0890030860900879</v>
+        <f t="shared" si="0"/>
+        <v>4.4575028584427407</v>
       </c>
       <c r="G40">
         <v>0.36976721882820129</v>
@@ -4797,13 +5172,13 @@
         <v>-1.3889377117156982</v>
       </c>
       <c r="S40">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T40">
         <v>-1.2443889379501343</v>
       </c>
       <c r="U40">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V40">
         <v>0.15380859375</v>
@@ -4833,7 +5208,7 @@
         <v>0.89940774440765381</v>
       </c>
       <c r="AE40">
-        <v>0.0065543390810489655</v>
+        <v>6.5543390810489655E-3</v>
       </c>
       <c r="AF40">
         <v>0</v>
@@ -4848,16 +5223,16 @@
         <v>0.97798269361853607</v>
       </c>
       <c r="AJ40">
-        <v>-0.020000552758574486</v>
+        <v>-2.0000552758574486E-2</v>
       </c>
       <c r="AK40">
-        <v>0.0065543390810489655</v>
+        <v>6.5543390810489655E-3</v>
       </c>
       <c r="AL40">
-        <v>-0.020779696470499154</v>
+        <v>-2.0779696470499154E-2</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:38">
       <c r="A41">
         <v>3.9000000000000004</v>
       </c>
@@ -4874,7 +5249,8 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0.022462422028183937</v>
+        <f t="shared" si="0"/>
+        <v>4.5639565138772351</v>
       </c>
       <c r="G41">
         <v>0.37337568402290344</v>
@@ -4913,13 +5289,13 @@
         <v>-1.3863018751144409</v>
       </c>
       <c r="S41">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="T41">
         <v>-1.244037389755249</v>
       </c>
       <c r="U41">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V41">
         <v>0.2252197265625</v>
@@ -4940,7 +5316,7 @@
         <v>0</v>
       </c>
       <c r="AB41">
-        <v>0.022462422028183937</v>
+        <v>2.2462422028183937E-2</v>
       </c>
       <c r="AC41">
         <v>0.37337568402290344</v>
@@ -4949,7 +5325,7 @@
         <v>0.91430544853210449</v>
       </c>
       <c r="AE41">
-        <v>0.0065059005282819271</v>
+        <v>6.5059005282819271E-3</v>
       </c>
       <c r="AF41">
         <v>0</v>
@@ -4964,15 +5340,17 @@
         <v>0.98129360313415537</v>
       </c>
       <c r="AJ41">
-        <v>-0.019999617710709572</v>
+        <v>-1.9999617710709572E-2</v>
       </c>
       <c r="AK41">
-        <v>0.0065059005282819271</v>
+        <v>6.5059005282819271E-3</v>
       </c>
       <c r="AL41">
-        <v>-0.020189598274230947</v>
+        <v>-2.0189598274230947E-2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>